<commit_message>
Updated Optimization code sor S-CO2
</commit_message>
<xml_diff>
--- a/Optimization Program/Optimization_Files/Optimization_Results.xlsx
+++ b/Optimization Program/Optimization_Files/Optimization_Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="8790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="8120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Run</t>
   </si>
@@ -62,25 +62,13 @@
     <t>Total Tubes</t>
   </si>
   <si>
-    <t>Outer Diameter of Curvature [m]</t>
-  </si>
-  <si>
-    <t>Height of Tube Bank [m]</t>
+    <t>Bundle Diameter [m]</t>
+  </si>
+  <si>
+    <t>Bundle Height [m]</t>
   </si>
   <si>
     <t>Total Surface Area [m^2]</t>
-  </si>
-  <si>
-    <t>Max Air Velocity [m/s]</t>
-  </si>
-  <si>
-    <t>Air Reynolds Number</t>
-  </si>
-  <si>
-    <t>U Coefficient [W/m^2*K]</t>
-  </si>
-  <si>
-    <t>Ideal Surface Area [m^2]</t>
   </si>
   <si>
     <t>Min F Factor</t>
@@ -444,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:W1"/>
+      <selection activeCell="L11" sqref="L11:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,17 +498,595 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.25</v>
+      </c>
+      <c r="C2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D2">
+        <v>1.256</v>
+      </c>
+      <c r="E2">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>31</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>0.33992615105408391</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>29</v>
+      </c>
+      <c r="L2">
+        <v>12136.5</v>
+      </c>
+      <c r="M2">
+        <v>2.2674603021081676</v>
+      </c>
+      <c r="N2">
+        <v>4.3601753408484667</v>
+      </c>
+      <c r="O2">
+        <v>3362.6710993468751</v>
+      </c>
+      <c r="P2">
+        <v>6.4024445451492733</v>
+      </c>
+      <c r="Q2">
+        <v>5.265108361920301E-2</v>
+      </c>
+      <c r="R2">
+        <v>88.612008145706156</v>
+      </c>
+      <c r="S2">
+        <v>0.79380399999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.18749999999999997</v>
+      </c>
+      <c r="C3">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.256</v>
+      </c>
+      <c r="E3">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>0.39175603553995719</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>25</v>
+      </c>
+      <c r="L3">
+        <v>7500</v>
+      </c>
+      <c r="M3">
+        <v>1.3661944710799143</v>
+      </c>
+      <c r="N3">
+        <v>3.6148745078418734</v>
+      </c>
+      <c r="O3">
+        <v>757.83590156053288</v>
+      </c>
+      <c r="P3">
+        <v>19.377665578097165</v>
+      </c>
+      <c r="Q3">
+        <v>5.4827318098696502E-2</v>
+      </c>
+      <c r="R3">
+        <v>421.19880568355376</v>
+      </c>
+      <c r="S3">
+        <v>0.29134119999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.18749999999999997</v>
+      </c>
+      <c r="C4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.256</v>
+      </c>
+      <c r="E4">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>0.33147421956225037</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>46</v>
+      </c>
+      <c r="L4">
+        <v>17388</v>
+      </c>
+      <c r="M4">
+        <v>1.3891916391245007</v>
+      </c>
+      <c r="N4">
+        <v>6.0159184510701156</v>
+      </c>
+      <c r="O4">
+        <v>1677.2251568705242</v>
+      </c>
+      <c r="P4">
+        <v>10.778058265684624</v>
+      </c>
+      <c r="Q4">
+        <v>3.2684320525875707E-2</v>
+      </c>
+      <c r="R4">
+        <v>87.989823635776432</v>
+      </c>
+      <c r="S4">
+        <v>0.36312159999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.18749999999999997</v>
+      </c>
+      <c r="C5">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.256</v>
+      </c>
+      <c r="E5">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>33</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>0.41110186809488913</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>42</v>
+      </c>
+      <c r="L5">
+        <v>15246</v>
+      </c>
+      <c r="M5">
+        <v>1.5484469361897781</v>
+      </c>
+      <c r="N5">
+        <v>5.0576495582421419</v>
+      </c>
+      <c r="O5">
+        <v>1698.8624321368623</v>
+      </c>
+      <c r="P5">
+        <v>10.485725795405774</v>
+      </c>
+      <c r="Q5">
+        <v>3.4486185948110294E-2</v>
+      </c>
+      <c r="R5">
+        <v>128.78787285990376</v>
+      </c>
+      <c r="S5">
+        <v>0.36312159999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.25</v>
+      </c>
+      <c r="C6">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.256</v>
+      </c>
+      <c r="E6">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>0.34472648891427154</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>53</v>
+      </c>
+      <c r="L6">
+        <v>19875</v>
+      </c>
+      <c r="M6">
+        <v>1.9899393778285428</v>
+      </c>
+      <c r="N6">
+        <v>12.60554412318255</v>
+      </c>
+      <c r="O6">
+        <v>6674.9331053974429</v>
+      </c>
+      <c r="P6">
+        <v>5.1325265128606947</v>
+      </c>
+      <c r="Q6">
+        <v>8.139168923949263E-3</v>
+      </c>
+      <c r="R6">
+        <v>44.309195210906317</v>
+      </c>
+      <c r="S6">
+        <v>0.65024319999999991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.18749999999999997</v>
+      </c>
+      <c r="C7">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D7">
+        <v>1.256</v>
+      </c>
+      <c r="E7">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>33</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>0.36449032982996987</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>29</v>
+      </c>
+      <c r="L7">
+        <v>10048.5</v>
+      </c>
+      <c r="M7">
+        <v>2.0294670596599396</v>
+      </c>
+      <c r="N7">
+        <v>3.4921865997386217</v>
+      </c>
+      <c r="O7">
+        <v>2605.7378642725771</v>
+      </c>
+      <c r="P7">
+        <v>6.1853609108037997</v>
+      </c>
+      <c r="Q7">
+        <v>0.10082537698206892</v>
+      </c>
+      <c r="R7">
+        <v>636.21288513412844</v>
+      </c>
+      <c r="S7">
+        <v>0.6502431999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0.12</v>
+      </c>
+      <c r="D8">
+        <v>1.256</v>
+      </c>
+      <c r="E8">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>36</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>0.52703293915563987</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>36</v>
+      </c>
+      <c r="L8">
+        <v>6480</v>
+      </c>
+      <c r="M8">
+        <v>1.9717234783112798</v>
+      </c>
+      <c r="N8">
+        <v>12.374960245711547</v>
+      </c>
+      <c r="O8">
+        <v>2457.6337537825543</v>
+      </c>
+      <c r="P8">
+        <v>20.46385086348997</v>
+      </c>
+      <c r="Q8">
+        <v>1.8001965127928067E-3</v>
+      </c>
+      <c r="R8">
+        <v>4.5879869743847186</v>
+      </c>
+      <c r="S8">
+        <v>0.45882879999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <v>0.12</v>
+      </c>
+      <c r="D9">
+        <v>1.256</v>
+      </c>
+      <c r="E9">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>37</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>0.39310789222321318</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>30</v>
+      </c>
+      <c r="L9">
+        <v>9990</v>
+      </c>
+      <c r="M9">
+        <v>2.2143117844464264</v>
+      </c>
+      <c r="N9">
+        <v>10.588749759843216</v>
+      </c>
+      <c r="O9">
+        <v>3757.2195720882855</v>
+      </c>
+      <c r="P9">
+        <v>12.388705800121697</v>
+      </c>
+      <c r="Q9">
+        <v>3.9699082543196967E-3</v>
+      </c>
+      <c r="R9">
+        <v>2.0939556914372486</v>
+      </c>
+      <c r="S9">
+        <v>0.71404799999999991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>0.12</v>
+      </c>
+      <c r="D10">
+        <v>1.256</v>
+      </c>
+      <c r="E10">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>33</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>0.31353728611535669</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>33</v>
+      </c>
+      <c r="L10">
+        <v>7623</v>
+      </c>
+      <c r="M10">
+        <v>1.7999513722307132</v>
+      </c>
+      <c r="N10">
+        <v>10.43198002679306</v>
+      </c>
+      <c r="O10">
+        <v>2319.0163200937195</v>
+      </c>
+      <c r="P10">
+        <v>18.0420180573505</v>
+      </c>
+      <c r="Q10">
+        <v>4.7161898798285858E-3</v>
+      </c>
+      <c r="R10">
+        <v>2.7490078120484234</v>
+      </c>
+      <c r="S10">
+        <v>0.58643839999999992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>0.12</v>
+      </c>
+      <c r="D11">
+        <v>1.256</v>
+      </c>
+      <c r="E11">
+        <v>1.4503038762043399</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>36</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>0.50706767806019315</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>43</v>
+      </c>
+      <c r="L11">
+        <v>10836</v>
+      </c>
+      <c r="M11">
+        <v>1.9317929561203862</v>
+      </c>
+      <c r="N11">
+        <v>11.118151886783259</v>
+      </c>
+      <c r="O11">
+        <v>3000.9302434898013</v>
+      </c>
+      <c r="P11">
+        <v>13.281178503810802</v>
+      </c>
+      <c r="Q11">
+        <v>3.3078880236565886E-3</v>
+      </c>
+      <c r="R11">
+        <v>5.0581524726810709</v>
+      </c>
+      <c r="S11">
+        <v>0.45882879999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>